<commit_message>
Update Holidays Excel file and import method and add more folders to gitignore
</commit_message>
<xml_diff>
--- a/Sistema de Gestao de Assiduidade/ExternalData/feriados.xlsx
+++ b/Sistema de Gestao de Assiduidade/ExternalData/feriados.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F62CB0-09BF-417F-91CD-E8B4DB2BDD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Dia dos Heróis Moçambicanos</t>
   </si>
@@ -73,13 +74,40 @@
   </si>
   <si>
     <t>Dia da Fraternidade universal</t>
+  </si>
+  <si>
+    <t>2016-01-01</t>
+  </si>
+  <si>
+    <t>2016-02-03</t>
+  </si>
+  <si>
+    <t>2016-04-07</t>
+  </si>
+  <si>
+    <t>2016-05-01</t>
+  </si>
+  <si>
+    <t>2016-06-25</t>
+  </si>
+  <si>
+    <t>2016-09-07</t>
+  </si>
+  <si>
+    <t>2016-09-25</t>
+  </si>
+  <si>
+    <t>2016-10-04</t>
+  </si>
+  <si>
+    <t>2016-12-25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -127,10 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -139,6 +164,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -185,7 +218,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,9 +250,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,6 +302,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -426,21 +495,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
     <col min="4" max="4" width="58.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -454,21 +523,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="5">
-        <v>42370</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="5">
-        <v>42403</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>
@@ -480,9 +549,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="5">
-        <v>42467</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
@@ -494,9 +563,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="5">
-        <v>42491</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -506,9 +575,9 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="5">
-        <v>42546</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -518,9 +587,9 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="5">
-        <v>42620</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
@@ -532,9 +601,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" customHeight="1">
-      <c r="A8" s="5">
-        <v>42638</v>
+    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
@@ -546,9 +615,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="5">
-        <v>42647</v>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
@@ -560,9 +629,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="5">
-        <v>42729</v>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
@@ -579,12 +648,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -592,12 +661,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>